<commit_message>
Add nopCommerce project files to Git
</commit_message>
<xml_diff>
--- a/src/test/resources/logs/inputData.xlsx
+++ b/src/test/resources/logs/inputData.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{373098D5-4CFA-4896-B07B-E4FA8616CEFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Akilbek\Montreal College IT\FINAL PROJECT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DBC91DB-4D2F-47C5-A10A-A0D85C5658CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="6576" xr2:uid="{6DE8DA25-A6AC-4C1E-A323-81556D2A6DE9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{6DE8DA25-A6AC-4C1E-A323-81556D2A6DE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>browser</t>
   </si>
@@ -36,6 +40,9 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -415,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC73648-BE4E-4647-8998-B3962594B6F5}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,6 +457,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>